<commit_message>
update reference to latest design, fix BOM
</commit_message>
<xml_diff>
--- a/legacy/arena_12-12/production_v2/BOM.xlsx
+++ b/legacy/arena_12-12/production_v2/BOM.xlsx
@@ -8,7 +8,8 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="BOM" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="BOM_BOTTOM (default)" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="BOM_TOP" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="105">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -238,6 +239,93 @@
     <t xml:space="preserve">J1;J2;J3;J4;J5;J6;J7;J8;J9;J10;J17;J19</t>
   </si>
   <si>
+    <t xml:space="preserve">CONN HDR 15POS 0.1 GOLD PCB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sullins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PPPC151LFBN-RC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S7048-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Any other connector with same specs is OK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONN PWR JACK 2X5.5MM SOLDER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CUI Devices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PJ-102A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CP-102A-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Footprint of connector and GERBER differ, but it should fit. Any other connector with same specs is OK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONN HEADER SMD 40POS 1.27MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CNC Tech</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3221-40-0300-00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1175-1750-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RN1;RN2;RN3;RN4;RN5;RN6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES ARRAY 8 RES 22 OHM 16SSOP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16SSOP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vishay Thin Film</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VSSR1603220JUF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VSSR16-22-JI-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alternative: VSSR1603220JTF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U1;U2;U3;U4;U5;U6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC TRANSLATION TXRX 5.5V 24TSSOP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24-TSSOP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Texas Instruments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SN74LVC8T245PWR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">296-18593-1-ND</t>
+  </si>
+  <si>
     <t xml:space="preserve">CONN HEADER VERT 15POS 2.54MM</t>
   </si>
   <si>
@@ -248,81 +336,6 @@
   </si>
   <si>
     <t xml:space="preserve">2057-PH1-15-UA-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Any other connector with same specs is OK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CONN PWR JACK 2X5.5MM SOLDER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CUI Devices</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PJ-102A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CP-102A-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Footprint of connector and GERBER differ, but it should fit. Any other connector with same specs is OK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CONN HEADER SMD 40POS 1.27MM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CNC Tech</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3221-40-0300-00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1175-1750-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RN1;RN2;RN3;RN4;RN5;RN6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RES ARRAY 8 RES 22 OHM 16SSOP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16SSOP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vishay Thin Film</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VSSR1603220JUF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VSSR16-22-JI-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alternative: VSSR1603220JTF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U1;U2;U3;U4;U5;U6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IC TRANSLATION TXRX 5.5V 24TSSOP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24-TSSOP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Texas Instruments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SN74LVC8T245PWR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">296-18593-1-ND</t>
   </si>
 </sst>
 </file>
@@ -446,7 +459,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -982,4 +995,558 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:Q20"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="81.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="53.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="1" width="53.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="86.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="1" width="53.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="34.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="51.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="11.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="13.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="10.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="128.57"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="3"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E14" s="4"/>
+      <c r="F14" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E16" s="4"/>
+      <c r="F16" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E20" s="4"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>